<commit_message>
added pivot chart to category worksheet
</commit_message>
<xml_diff>
--- a/crowdfunding.xlsx
+++ b/crowdfunding.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremytallant/Desktop/My_Repositories/excel-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88D554-B7A3-AA4D-B98C-9E8A24975D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB74ED70-12E1-8C48-B238-6C60B7A24C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -26875,7 +26875,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2255D7A2-10BD-604E-BB85-48BED9FFBD2D}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2255D7A2-10BD-604E-BB85-48BED9FFBD2D}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:F14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -26990,6 +26990,104 @@
   <dataFields count="1">
     <dataField name="Count of outcome" fld="6" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="8">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -27302,7 +27400,7 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -87410,7 +87508,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -87420,6 +87518,11 @@
     <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added pivot chart 2 to excel file
</commit_message>
<xml_diff>
--- a/crowdfunding.xlsx
+++ b/crowdfunding.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremytallant/Desktop/My_Repositories/excel-challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE72537F-B48C-AF40-8CC4-E88D3B5A9A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FF81BF-4D56-F14B-BBB6-D9443B13C565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crowdfunding" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId4"/>
+    <pivotCache cacheId="12" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -6732,7 +6732,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6749,7 +6749,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7765,6 +7764,1168 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[crowdfunding.xlsx]Sub-Category!PivotTable3</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="0070C0"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sub-Category'!$B$4:$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>canceled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sub-Category'!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>audio</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>documentary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>drama</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>electric music</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fiction</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>food trucks</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>indie rock</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jazz</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>metal</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mobile games</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>nonfiction</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>photography books</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>plays</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>radio &amp; podcasts</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>rock</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>science fiction</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>shorts</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>television</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>translations</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>video games</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>wearables</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>web</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>world music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sub-Category'!$B$6:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCFD-E94C-A8B8-0B0170BE5879}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sub-Category'!$C$4:$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sub-Category'!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>audio</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>documentary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>drama</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>electric music</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fiction</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>food trucks</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>indie rock</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jazz</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>metal</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mobile games</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>nonfiction</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>photography books</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>plays</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>radio &amp; podcasts</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>rock</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>science fiction</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>shorts</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>television</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>translations</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>video games</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>wearables</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>web</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>world music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sub-Category'!$C$6:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FCFD-E94C-A8B8-0B0170BE5879}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sub-Category'!$D$4:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>live</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sub-Category'!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>audio</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>documentary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>drama</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>electric music</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fiction</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>food trucks</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>indie rock</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jazz</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>metal</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mobile games</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>nonfiction</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>photography books</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>plays</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>radio &amp; podcasts</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>rock</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>science fiction</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>shorts</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>television</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>translations</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>video games</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>wearables</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>web</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>world music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sub-Category'!$D$6:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FCFD-E94C-A8B8-0B0170BE5879}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sub-Category'!$E$4:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>successful</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sub-Category'!$A$6:$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>animation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>audio</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>documentary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>drama</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>electric music</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fiction</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>food trucks</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>indie rock</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jazz</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>metal</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>mobile games</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>nonfiction</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>photography books</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>plays</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>radio &amp; podcasts</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>rock</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>science fiction</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>shorts</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>television</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>translations</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>video games</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>wearables</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>web</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>world music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sub-Category'!$E$6:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FCFD-E94C-A8B8-0B0170BE5879}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="100"/>
+        <c:axId val="439688688"/>
+        <c:axId val="439690688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="439688688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="439690688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="439690688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="439688688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -7802,7 +8963,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8346,6 +10050,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5A146CF-DA2C-FDDC-5732-FB6C18357560}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45267.199105902779" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1000" xr:uid="{EE6F355A-EAB1-9249-BE0E-A1E711F5DCDA}">
   <cacheSource type="worksheet">
@@ -28469,7 +30214,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2255D7A2-10BD-604E-BB85-48BED9FFBD2D}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2255D7A2-10BD-604E-BB85-48BED9FFBD2D}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:F14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -28752,7 +30497,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BBC7E2E6-F062-7E46-B48C-10A382FA6716}" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BBC7E2E6-F062-7E46-B48C-10A382FA6716}" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A4:F30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -28941,6 +30686,56 @@
   <dataFields count="1">
     <dataField name="Count of outcome" fld="6" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -89418,19 +91213,19 @@
       <c r="A5" s="7" t="s">
         <v>2035</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5">
         <v>11</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>60</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>102</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5">
         <v>178</v>
       </c>
     </row>
@@ -89438,17 +91233,16 @@
       <c r="A6" s="7" t="s">
         <v>2036</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>22</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6">
         <v>46</v>
       </c>
     </row>
@@ -89456,19 +91250,19 @@
       <c r="A7" s="7" t="s">
         <v>2037</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>23</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>21</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7">
         <v>48</v>
       </c>
     </row>
@@ -89476,13 +91270,10 @@
       <c r="A8" s="7" t="s">
         <v>2038</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8">
         <v>4</v>
       </c>
     </row>
@@ -89490,17 +91281,16 @@
       <c r="A9" s="7" t="s">
         <v>2039</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>10</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>66</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>99</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9">
         <v>175</v>
       </c>
     </row>
@@ -89508,19 +91298,19 @@
       <c r="A10" s="7" t="s">
         <v>2040</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>11</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>26</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10">
         <v>42</v>
       </c>
     </row>
@@ -89528,19 +91318,19 @@
       <c r="A11" s="7" t="s">
         <v>2041</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>24</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>40</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11">
         <v>67</v>
       </c>
     </row>
@@ -89548,19 +91338,19 @@
       <c r="A12" s="7" t="s">
         <v>2042</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>28</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>64</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12">
         <v>96</v>
       </c>
     </row>
@@ -89568,19 +91358,19 @@
       <c r="A13" s="7" t="s">
         <v>2043</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>23</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>132</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>187</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13">
         <v>344</v>
       </c>
     </row>
@@ -89588,19 +91378,19 @@
       <c r="A14" s="7" t="s">
         <v>2044</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <v>57</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>364</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14">
         <v>14</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>565</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14">
         <v>1000</v>
       </c>
     </row>
@@ -89614,7 +91404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D6225F-9956-CA4F-B951-80F36210E144}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -89673,19 +91465,19 @@
       <c r="A6" s="7" t="s">
         <v>2047</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>21</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6">
         <v>34</v>
       </c>
     </row>
@@ -89693,13 +91485,10 @@
       <c r="A7" s="7" t="s">
         <v>2048</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7">
         <v>4</v>
       </c>
     </row>
@@ -89707,19 +91496,19 @@
       <c r="A8" s="7" t="s">
         <v>2049</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>21</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>34</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8">
         <v>60</v>
       </c>
     </row>
@@ -89727,19 +91516,19 @@
       <c r="A9" s="7" t="s">
         <v>2050</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>12</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>22</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9">
         <v>37</v>
       </c>
     </row>
@@ -89747,15 +91536,13 @@
       <c r="A10" s="7" t="s">
         <v>2051</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>10</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10">
         <v>18</v>
       </c>
     </row>
@@ -89763,17 +91550,16 @@
       <c r="A11" s="7" t="s">
         <v>2052</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>7</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>9</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11">
         <v>17</v>
       </c>
     </row>
@@ -89781,17 +91567,16 @@
       <c r="A12" s="7" t="s">
         <v>2053</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>20</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>22</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12">
         <v>46</v>
       </c>
     </row>
@@ -89799,17 +91584,16 @@
       <c r="A13" s="7" t="s">
         <v>2054</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>19</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>23</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13">
         <v>45</v>
       </c>
     </row>
@@ -89817,17 +91601,16 @@
       <c r="A14" s="7" t="s">
         <v>2055</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>10</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14">
         <v>17</v>
       </c>
     </row>
@@ -89835,15 +91618,13 @@
       <c r="A15" s="7" t="s">
         <v>2056</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>4</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15">
         <v>7</v>
       </c>
     </row>
@@ -89851,17 +91632,16 @@
       <c r="A16" s="7" t="s">
         <v>2057</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8">
+      <c r="C16">
         <v>8</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>4</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16">
         <v>13</v>
       </c>
     </row>
@@ -89869,19 +91649,19 @@
       <c r="A17" s="7" t="s">
         <v>2058</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17">
         <v>6</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>13</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17">
         <v>21</v>
       </c>
     </row>
@@ -89889,19 +91669,19 @@
       <c r="A18" s="7" t="s">
         <v>2059</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18">
         <v>11</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18">
         <v>26</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18">
         <v>42</v>
       </c>
     </row>
@@ -89909,19 +91689,19 @@
       <c r="A19" s="7" t="s">
         <v>2060</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19">
         <v>23</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19">
         <v>132</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19">
         <v>187</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19">
         <v>344</v>
       </c>
     </row>
@@ -89929,15 +91709,13 @@
       <c r="A20" s="7" t="s">
         <v>2061</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8">
+      <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8">
+      <c r="E20">
         <v>4</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20">
         <v>8</v>
       </c>
     </row>
@@ -89945,17 +91723,16 @@
       <c r="A21" s="7" t="s">
         <v>2062</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21">
         <v>30</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8">
+      <c r="E21">
         <v>49</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21">
         <v>85</v>
       </c>
     </row>
@@ -89963,15 +91740,13 @@
       <c r="A22" s="7" t="s">
         <v>2063</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8">
+      <c r="C22">
         <v>9</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8">
+      <c r="E22">
         <v>5</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22">
         <v>14</v>
       </c>
     </row>
@@ -89979,19 +91754,19 @@
       <c r="A23" s="7" t="s">
         <v>2064</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23">
         <v>5</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23">
         <v>9</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23">
         <v>16</v>
       </c>
     </row>
@@ -89999,17 +91774,16 @@
       <c r="A24" s="7" t="s">
         <v>2065</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24">
         <v>3</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8">
+      <c r="E24">
         <v>11</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24">
         <v>17</v>
       </c>
     </row>
@@ -90017,15 +91791,13 @@
       <c r="A25" s="7" t="s">
         <v>2066</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8">
+      <c r="C25">
         <v>7</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8">
+      <c r="E25">
         <v>14</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25">
         <v>21</v>
       </c>
     </row>
@@ -90033,19 +91805,19 @@
       <c r="A26" s="7" t="s">
         <v>2067</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26">
         <v>15</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26">
         <v>17</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26">
         <v>35</v>
       </c>
     </row>
@@ -90053,17 +91825,16 @@
       <c r="A27" s="7" t="s">
         <v>2068</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8">
+      <c r="C27">
         <v>16</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27">
         <v>28</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27">
         <v>45</v>
       </c>
     </row>
@@ -90071,19 +91842,19 @@
       <c r="A28" s="7" t="s">
         <v>2069</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28">
         <v>12</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28">
         <v>36</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28">
         <v>51</v>
       </c>
     </row>
@@ -90091,13 +91862,10 @@
       <c r="A29" s="7" t="s">
         <v>2070</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8">
+      <c r="E29">
         <v>3</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29">
         <v>3</v>
       </c>
     </row>
@@ -90105,23 +91873,24 @@
       <c r="A30" s="7" t="s">
         <v>2044</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30">
         <v>57</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30">
         <v>364</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30">
         <v>14</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30">
         <v>565</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>